<commit_message>
feat: add kobo workflow and minor edit to stems app
</commit_message>
<xml_diff>
--- a/app/desfert_stems.xlsx
+++ b/app/desfert_stems.xlsx
@@ -117,7 +117,7 @@
     <t xml:space="preserve">plot_id</t>
   </si>
   <si>
-    <t xml:space="preserve">plod ID</t>
+    <t xml:space="preserve">plot ID</t>
   </si>
   <si>
     <t xml:space="preserve">site=${site}</t>
@@ -177,10 +177,10 @@
     <t xml:space="preserve">(m)</t>
   </si>
   <si>
-    <t xml:space="preserve">. &gt;= 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">must be a positive number</t>
+    <t xml:space="preserve">. &gt;= 0 and .&lt;5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">must be a positive number in units of m</t>
   </si>
   <si>
     <t xml:space="preserve">plant_dimension_e_w</t>
@@ -874,7 +874,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="44.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="55.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="35.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.79"/>
@@ -2509,7 +2509,7 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.08"/>
@@ -2543,7 +2543,7 @@
       </c>
       <c r="D2" s="1" t="str">
         <f aca="true">CONCATENATE(YEAR(TODAY()),TEXT(MONTH(TODAY()),"00"),TEXT(DAY(TODAY()),"00"),TEXT(HOUR(NOW()),"00"),TEXT(MINUTE(NOW()),"00"))</f>
-        <v>202204301401</v>
+        <v>202206271247</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>170</v>

</xml_diff>